<commit_message>
Calendario, Insertar Fechas Feriados, Reserva desde Busqueda Ambiente
</commit_message>
<xml_diff>
--- a/reservaTis/storage/archivos/calendario.xlsx
+++ b/reservaTis/storage/archivos/calendario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gunnar/Documents/Estudiante/Tis/R2D2/reservaTis/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gunnar/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,25 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="33">
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="35">
   <si>
     <t>Venta de matriculas 1-2017</t>
   </si>
@@ -129,6 +111,30 @@
   </si>
   <si>
     <t>actividad</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sabado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>MIercoles</t>
   </si>
 </sst>
 </file>
@@ -516,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="B313" sqref="B313:B319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,22 +533,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -550,11 +556,11 @@
         <v>42783</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>41255</v>
@@ -568,7 +574,7 @@
         <v>42784</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -584,7 +590,7 @@
         <v>42785</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -600,13 +606,13 @@
         <v>42786</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>41258</v>
@@ -620,11 +626,11 @@
         <v>42787</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>41259</v>
@@ -638,11 +644,11 @@
         <v>42788</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
         <v>41260</v>
@@ -656,11 +662,11 @@
         <v>42789</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>41261</v>
@@ -674,11 +680,11 @@
         <v>42790</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>41262</v>
@@ -692,7 +698,7 @@
         <v>42791</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="2"/>
@@ -708,7 +714,7 @@
         <v>42792</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -724,7 +730,7 @@
         <v>42793</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -742,7 +748,7 @@
         <v>42794</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="2"/>
@@ -758,11 +764,11 @@
         <v>42795</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E14" s="5">
         <v>41267</v>
@@ -776,11 +782,11 @@
         <v>42796</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5">
         <v>41268</v>
@@ -794,11 +800,11 @@
         <v>42797</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E16" s="5">
         <v>41269</v>
@@ -812,7 +818,7 @@
         <v>42798</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="2"/>
@@ -828,7 +834,7 @@
         <v>42799</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -844,7 +850,7 @@
         <v>42800</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
@@ -862,7 +868,7 @@
         <v>42801</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="2"/>
@@ -878,7 +884,7 @@
         <v>42802</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="2"/>
@@ -894,11 +900,11 @@
         <v>42803</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E22" s="5">
         <v>41275</v>
@@ -912,11 +918,11 @@
         <v>42804</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E23" s="5">
         <v>41276</v>
@@ -930,7 +936,7 @@
         <v>42805</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="2"/>
@@ -946,7 +952,7 @@
         <v>42806</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -962,13 +968,13 @@
         <v>42807</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E26" s="5">
         <v>41279</v>
@@ -982,7 +988,7 @@
         <v>42808</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="2"/>
@@ -998,7 +1004,7 @@
         <v>42809</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="2"/>
@@ -1014,7 +1020,7 @@
         <v>42810</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="2"/>
@@ -1030,7 +1036,7 @@
         <v>42811</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="2"/>
@@ -1046,7 +1052,7 @@
         <v>42812</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="2"/>
@@ -1062,7 +1068,7 @@
         <v>42813</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1078,13 +1084,13 @@
         <v>42814</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C33" s="6">
         <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E33" s="5">
         <v>41286</v>
@@ -1098,7 +1104,7 @@
         <v>42815</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="2"/>
@@ -1114,7 +1120,7 @@
         <v>42816</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="2"/>
@@ -1130,11 +1136,11 @@
         <v>42817</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E36" s="5">
         <v>41289</v>
@@ -1148,7 +1154,7 @@
         <v>42818</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="2"/>
@@ -1164,7 +1170,7 @@
         <v>42819</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="2"/>
@@ -1180,7 +1186,7 @@
         <v>42820</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1196,7 +1202,7 @@
         <v>42821</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C40" s="6">
         <v>5</v>
@@ -1214,7 +1220,7 @@
         <v>42822</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="2"/>
@@ -1230,7 +1236,7 @@
         <v>42823</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="2"/>
@@ -1246,7 +1252,7 @@
         <v>42824</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="2"/>
@@ -1262,7 +1268,7 @@
         <v>42825</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="2"/>
@@ -1278,7 +1284,7 @@
         <v>42826</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="2"/>
@@ -1294,7 +1300,7 @@
         <v>42827</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1310,13 +1316,13 @@
         <v>42828</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C47" s="6">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E47" s="5">
         <v>43080</v>
@@ -1330,7 +1336,7 @@
         <v>42829</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="2"/>
@@ -1346,7 +1352,7 @@
         <v>42830</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="2"/>
@@ -1362,7 +1368,7 @@
         <v>42831</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="2"/>
@@ -1378,7 +1384,7 @@
         <v>42832</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="2"/>
@@ -1394,7 +1400,7 @@
         <v>42833</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="2"/>
@@ -1410,7 +1416,7 @@
         <v>42834</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -1426,7 +1432,7 @@
         <v>42835</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C54" s="6">
         <v>7</v>
@@ -1444,7 +1450,7 @@
         <v>42836</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="2"/>
@@ -1460,7 +1466,7 @@
         <v>42837</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="2"/>
@@ -1476,7 +1482,7 @@
         <v>42838</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="2"/>
@@ -1492,11 +1498,11 @@
         <v>42839</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E58" s="5">
         <v>43091</v>
@@ -1510,7 +1516,7 @@
         <v>42840</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="2"/>
@@ -1526,7 +1532,7 @@
         <v>42841</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1542,13 +1548,13 @@
         <v>42842</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C61" s="6">
         <v>8</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E61" s="5">
         <v>43094</v>
@@ -1562,7 +1568,7 @@
         <v>42843</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="2"/>
@@ -1578,7 +1584,7 @@
         <v>42844</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="2"/>
@@ -1594,7 +1600,7 @@
         <v>42845</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="2"/>
@@ -1610,7 +1616,7 @@
         <v>42846</v>
       </c>
       <c r="B65" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="2"/>
@@ -1626,7 +1632,7 @@
         <v>42847</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="2"/>
@@ -1642,7 +1648,7 @@
         <v>42848</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -1658,7 +1664,7 @@
         <v>42849</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C68" s="6">
         <v>9</v>
@@ -1676,7 +1682,7 @@
         <v>42850</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="2"/>
@@ -1692,7 +1698,7 @@
         <v>42851</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="2"/>
@@ -1708,7 +1714,7 @@
         <v>42852</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="2"/>
@@ -1724,7 +1730,7 @@
         <v>42853</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="2"/>
@@ -1740,11 +1746,11 @@
         <v>42854</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E73" s="5">
         <v>43106</v>
@@ -1758,7 +1764,7 @@
         <v>42855</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -1774,7 +1780,7 @@
         <v>42856</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C75" s="6">
         <v>10</v>
@@ -1792,7 +1798,7 @@
         <v>42857</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="2"/>
@@ -1808,7 +1814,7 @@
         <v>42858</v>
       </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="2"/>
@@ -1824,7 +1830,7 @@
         <v>42859</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="2"/>
@@ -1840,7 +1846,7 @@
         <v>42860</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="2"/>
@@ -1856,7 +1862,7 @@
         <v>42861</v>
       </c>
       <c r="B80" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="2"/>
@@ -1872,7 +1878,7 @@
         <v>42862</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -1888,7 +1894,7 @@
         <v>42863</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C82" s="6">
         <v>11</v>
@@ -1906,7 +1912,7 @@
         <v>42864</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="2"/>
@@ -1922,7 +1928,7 @@
         <v>42865</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="2"/>
@@ -1938,7 +1944,7 @@
         <v>42866</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="2"/>
@@ -1954,7 +1960,7 @@
         <v>42867</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="2"/>
@@ -1970,7 +1976,7 @@
         <v>42868</v>
       </c>
       <c r="B87" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="2"/>
@@ -1986,7 +1992,7 @@
         <v>42869</v>
       </c>
       <c r="B88" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -2002,7 +2008,7 @@
         <v>42870</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C89" s="6">
         <v>12</v>
@@ -2020,7 +2026,7 @@
         <v>42871</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="2"/>
@@ -2036,7 +2042,7 @@
         <v>42872</v>
       </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="2"/>
@@ -2052,7 +2058,7 @@
         <v>42873</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="2"/>
@@ -2068,7 +2074,7 @@
         <v>42874</v>
       </c>
       <c r="B93" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="2"/>
@@ -2084,7 +2090,7 @@
         <v>42875</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="2"/>
@@ -2100,7 +2106,7 @@
         <v>42876</v>
       </c>
       <c r="B95" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -2116,7 +2122,7 @@
         <v>42877</v>
       </c>
       <c r="B96" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C96" s="6">
         <v>13</v>
@@ -2134,7 +2140,7 @@
         <v>42878</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="2"/>
@@ -2150,7 +2156,7 @@
         <v>42879</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="2"/>
@@ -2166,7 +2172,7 @@
         <v>42880</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="2"/>
@@ -2182,7 +2188,7 @@
         <v>42881</v>
       </c>
       <c r="B100" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="2"/>
@@ -2198,7 +2204,7 @@
         <v>42882</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="2"/>
@@ -2214,7 +2220,7 @@
         <v>42883</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -2230,7 +2236,7 @@
         <v>42884</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C103" s="6">
         <v>14</v>
@@ -2248,7 +2254,7 @@
         <v>42885</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="2"/>
@@ -2264,7 +2270,7 @@
         <v>42886</v>
       </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="2"/>
@@ -2280,7 +2286,7 @@
         <v>42887</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="2"/>
@@ -2296,7 +2302,7 @@
         <v>42888</v>
       </c>
       <c r="B107" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="2"/>
@@ -2312,7 +2318,7 @@
         <v>42889</v>
       </c>
       <c r="B108" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="2"/>
@@ -2328,7 +2334,7 @@
         <v>42890</v>
       </c>
       <c r="B109" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -2344,7 +2350,7 @@
         <v>42891</v>
       </c>
       <c r="B110" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C110" s="6">
         <v>15</v>
@@ -2362,7 +2368,7 @@
         <v>42892</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="2"/>
@@ -2378,7 +2384,7 @@
         <v>42893</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="2"/>
@@ -2394,11 +2400,11 @@
         <v>42894</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E113" s="5">
         <v>43146</v>
@@ -2412,7 +2418,7 @@
         <v>42895</v>
       </c>
       <c r="B114" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114" s="2"/>
@@ -2428,7 +2434,7 @@
         <v>42896</v>
       </c>
       <c r="B115" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="2"/>
@@ -2444,7 +2450,7 @@
         <v>42897</v>
       </c>
       <c r="B116" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -2460,7 +2466,7 @@
         <v>42898</v>
       </c>
       <c r="B117" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C117" s="6">
         <v>16</v>
@@ -2478,7 +2484,7 @@
         <v>42899</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118" s="2"/>
@@ -2494,7 +2500,7 @@
         <v>42900</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C119" s="7"/>
       <c r="D119" s="2"/>
@@ -2510,7 +2516,7 @@
         <v>42901</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120" s="2"/>
@@ -2526,7 +2532,7 @@
         <v>42902</v>
       </c>
       <c r="B121" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121" s="2"/>
@@ -2542,7 +2548,7 @@
         <v>42903</v>
       </c>
       <c r="B122" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C122" s="8"/>
       <c r="D122" s="2"/>
@@ -2558,7 +2564,7 @@
         <v>42904</v>
       </c>
       <c r="B123" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -2574,7 +2580,7 @@
         <v>42905</v>
       </c>
       <c r="B124" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C124" s="6">
         <v>17</v>
@@ -2592,11 +2598,11 @@
         <v>42906</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C125" s="7"/>
       <c r="D125" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E125" s="5">
         <v>43158</v>
@@ -2610,11 +2616,11 @@
         <v>42907</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C126" s="7"/>
       <c r="D126" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E126" s="5">
         <v>43159</v>
@@ -2628,7 +2634,7 @@
         <v>42908</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C127" s="7"/>
       <c r="D127" s="2"/>
@@ -2644,7 +2650,7 @@
         <v>42909</v>
       </c>
       <c r="B128" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C128" s="7"/>
       <c r="D128" s="2"/>
@@ -2660,7 +2666,7 @@
         <v>42910</v>
       </c>
       <c r="B129" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="2"/>
@@ -2676,7 +2682,7 @@
         <v>42911</v>
       </c>
       <c r="B130" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -2692,7 +2698,7 @@
         <v>42912</v>
       </c>
       <c r="B131" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C131" s="6">
         <v>18</v>
@@ -2710,7 +2716,7 @@
         <v>42913</v>
       </c>
       <c r="B132" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C132" s="7"/>
       <c r="D132" s="2"/>
@@ -2726,11 +2732,11 @@
         <v>42914</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C133" s="7"/>
       <c r="D133" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E133" s="5">
         <v>43166</v>
@@ -2744,7 +2750,7 @@
         <v>42915</v>
       </c>
       <c r="B134" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C134" s="7"/>
       <c r="D134" s="2"/>
@@ -2760,7 +2766,7 @@
         <v>42916</v>
       </c>
       <c r="B135" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C135" s="7"/>
       <c r="D135" s="2"/>
@@ -2776,7 +2782,7 @@
         <v>42917</v>
       </c>
       <c r="B136" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C136" s="8"/>
       <c r="D136" s="2"/>
@@ -2792,7 +2798,7 @@
         <v>42918</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -2808,7 +2814,7 @@
         <v>42919</v>
       </c>
       <c r="B138" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C138" s="6">
         <v>19</v>
@@ -2826,7 +2832,7 @@
         <v>42920</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C139" s="7"/>
       <c r="D139" s="2"/>
@@ -2842,7 +2848,7 @@
         <v>42921</v>
       </c>
       <c r="B140" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C140" s="7"/>
       <c r="D140" s="2"/>
@@ -2858,7 +2864,7 @@
         <v>42922</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C141" s="7"/>
       <c r="D141" s="2"/>
@@ -2874,7 +2880,7 @@
         <v>42923</v>
       </c>
       <c r="B142" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C142" s="7"/>
       <c r="D142" s="2"/>
@@ -2890,7 +2896,7 @@
         <v>42924</v>
       </c>
       <c r="B143" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C143" s="8"/>
       <c r="D143" s="2"/>
@@ -2906,7 +2912,7 @@
         <v>42925</v>
       </c>
       <c r="B144" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -2922,7 +2928,7 @@
         <v>42926</v>
       </c>
       <c r="B145" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C145" s="6">
         <v>20</v>
@@ -2940,11 +2946,11 @@
         <v>42927</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C146" s="7"/>
       <c r="D146" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E146" s="5">
         <v>43179</v>
@@ -2958,11 +2964,11 @@
         <v>42928</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C147" s="7"/>
       <c r="D147" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E147" s="5">
         <v>43180</v>
@@ -2976,11 +2982,11 @@
         <v>42929</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C148" s="7"/>
       <c r="D148" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E148" s="5">
         <v>43181</v>
@@ -2994,11 +3000,11 @@
         <v>42930</v>
       </c>
       <c r="B149" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C149" s="7"/>
       <c r="D149" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E149" s="5">
         <v>43182</v>
@@ -3012,7 +3018,7 @@
         <v>42931</v>
       </c>
       <c r="B150" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C150" s="8"/>
       <c r="D150" s="2"/>
@@ -3028,7 +3034,7 @@
         <v>42932</v>
       </c>
       <c r="B151" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
@@ -3044,13 +3050,13 @@
         <v>42933</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C152" s="6">
         <v>21</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E152" s="5">
         <v>43185</v>
@@ -3064,7 +3070,7 @@
         <v>42934</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C153" s="7"/>
       <c r="D153" s="2"/>
@@ -3080,7 +3086,7 @@
         <v>42935</v>
       </c>
       <c r="B154" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C154" s="7"/>
       <c r="D154" s="2"/>
@@ -3096,7 +3102,7 @@
         <v>42936</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C155" s="7"/>
       <c r="D155" s="2"/>
@@ -3112,7 +3118,7 @@
         <v>42937</v>
       </c>
       <c r="B156" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C156" s="7"/>
       <c r="D156" s="2"/>
@@ -3128,7 +3134,7 @@
         <v>42938</v>
       </c>
       <c r="B157" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="2"/>
@@ -3144,7 +3150,7 @@
         <v>42939</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -3160,7 +3166,7 @@
         <v>42940</v>
       </c>
       <c r="B159" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C159" s="6">
         <v>22</v>
@@ -3178,7 +3184,7 @@
         <v>42941</v>
       </c>
       <c r="B160" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C160" s="7"/>
       <c r="D160" s="2"/>
@@ -3194,7 +3200,7 @@
         <v>42942</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C161" s="7"/>
       <c r="D161" s="2"/>
@@ -3210,7 +3216,7 @@
         <v>42943</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C162" s="7"/>
       <c r="D162" s="2"/>
@@ -3226,7 +3232,7 @@
         <v>42944</v>
       </c>
       <c r="B163" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C163" s="7"/>
       <c r="D163" s="2"/>
@@ -3242,7 +3248,7 @@
         <v>42945</v>
       </c>
       <c r="B164" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C164" s="8"/>
       <c r="D164" s="2"/>
@@ -3258,7 +3264,7 @@
         <v>42946</v>
       </c>
       <c r="B165" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -3274,7 +3280,7 @@
         <v>42947</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C166" s="6">
         <v>23</v>
@@ -3292,7 +3298,7 @@
         <v>42948</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C167" s="7"/>
       <c r="D167" s="2"/>
@@ -3308,7 +3314,7 @@
         <v>42949</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C168" s="7"/>
       <c r="D168" s="2"/>
@@ -3324,7 +3330,7 @@
         <v>42950</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C169" s="7"/>
       <c r="D169" s="2"/>
@@ -3340,7 +3346,7 @@
         <v>42951</v>
       </c>
       <c r="B170" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C170" s="7"/>
       <c r="D170" s="2"/>
@@ -3356,7 +3362,7 @@
         <v>42952</v>
       </c>
       <c r="B171" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C171" s="8"/>
       <c r="D171" s="2"/>
@@ -3372,7 +3378,7 @@
         <v>42953</v>
       </c>
       <c r="B172" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -3388,13 +3394,13 @@
         <v>42954</v>
       </c>
       <c r="B173" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C173" s="6">
         <v>24</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E173" s="5">
         <v>43206</v>
@@ -3408,11 +3414,11 @@
         <v>42955</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C174" s="7"/>
       <c r="D174" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E174" s="5">
         <v>43207</v>
@@ -3426,7 +3432,7 @@
         <v>42956</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C175" s="7"/>
       <c r="D175" s="2"/>
@@ -3442,7 +3448,7 @@
         <v>42957</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C176" s="7"/>
       <c r="D176" s="2"/>
@@ -3458,7 +3464,7 @@
         <v>42958</v>
       </c>
       <c r="B177" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C177" s="7"/>
       <c r="D177" s="2"/>
@@ -3474,7 +3480,7 @@
         <v>42959</v>
       </c>
       <c r="B178" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="2"/>
@@ -3490,7 +3496,7 @@
         <v>42960</v>
       </c>
       <c r="B179" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
@@ -3506,7 +3512,7 @@
         <v>42961</v>
       </c>
       <c r="B180" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C180" s="6">
         <v>25</v>
@@ -3524,7 +3530,7 @@
         <v>42962</v>
       </c>
       <c r="B181" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C181" s="7"/>
       <c r="D181" s="2"/>
@@ -3540,7 +3546,7 @@
         <v>42963</v>
       </c>
       <c r="B182" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C182" s="7"/>
       <c r="D182" s="2"/>
@@ -3556,7 +3562,7 @@
         <v>42964</v>
       </c>
       <c r="B183" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C183" s="7"/>
       <c r="D183" s="2"/>
@@ -3572,7 +3578,7 @@
         <v>42965</v>
       </c>
       <c r="B184" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C184" s="7"/>
       <c r="D184" s="2"/>
@@ -3588,7 +3594,7 @@
         <v>42966</v>
       </c>
       <c r="B185" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="2"/>
@@ -3604,7 +3610,7 @@
         <v>42967</v>
       </c>
       <c r="B186" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
@@ -3620,7 +3626,7 @@
         <v>42968</v>
       </c>
       <c r="B187" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C187" s="6">
         <v>26</v>
@@ -3638,7 +3644,7 @@
         <v>42969</v>
       </c>
       <c r="B188" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C188" s="7"/>
       <c r="D188" s="2"/>
@@ -3654,7 +3660,7 @@
         <v>42970</v>
       </c>
       <c r="B189" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C189" s="7"/>
       <c r="D189" s="2"/>
@@ -3670,7 +3676,7 @@
         <v>42971</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C190" s="7"/>
       <c r="D190" s="2"/>
@@ -3686,7 +3692,7 @@
         <v>42972</v>
       </c>
       <c r="B191" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C191" s="7"/>
       <c r="D191" s="2"/>
@@ -3702,7 +3708,7 @@
         <v>42973</v>
       </c>
       <c r="B192" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C192" s="8"/>
       <c r="D192" s="2"/>
@@ -3718,7 +3724,7 @@
         <v>42974</v>
       </c>
       <c r="B193" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -3734,7 +3740,7 @@
         <v>42975</v>
       </c>
       <c r="B194" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C194" s="6">
         <v>27</v>
@@ -3752,7 +3758,7 @@
         <v>42976</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C195" s="7"/>
       <c r="D195" s="2"/>
@@ -3768,7 +3774,7 @@
         <v>42977</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C196" s="7"/>
       <c r="D196" s="2"/>
@@ -3784,7 +3790,7 @@
         <v>42978</v>
       </c>
       <c r="B197" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C197" s="7"/>
       <c r="D197" s="2"/>
@@ -3800,7 +3806,7 @@
         <v>42979</v>
       </c>
       <c r="B198" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C198" s="7"/>
       <c r="D198" s="2"/>
@@ -3816,7 +3822,7 @@
         <v>42980</v>
       </c>
       <c r="B199" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C199" s="8"/>
       <c r="D199" s="2"/>
@@ -3832,7 +3838,7 @@
         <v>42981</v>
       </c>
       <c r="B200" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
@@ -3848,7 +3854,7 @@
         <v>42982</v>
       </c>
       <c r="B201" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C201" s="6">
         <v>28</v>
@@ -3866,7 +3872,7 @@
         <v>42983</v>
       </c>
       <c r="B202" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C202" s="7"/>
       <c r="D202" s="2"/>
@@ -3882,7 +3888,7 @@
         <v>42984</v>
       </c>
       <c r="B203" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C203" s="7"/>
       <c r="D203" s="2"/>
@@ -3898,7 +3904,7 @@
         <v>42985</v>
       </c>
       <c r="B204" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C204" s="7"/>
       <c r="D204" s="2"/>
@@ -3914,7 +3920,7 @@
         <v>42986</v>
       </c>
       <c r="B205" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C205" s="7"/>
       <c r="D205" s="2"/>
@@ -3930,7 +3936,7 @@
         <v>42987</v>
       </c>
       <c r="B206" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C206" s="8"/>
       <c r="D206" s="2"/>
@@ -3946,7 +3952,7 @@
         <v>42988</v>
       </c>
       <c r="B207" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
@@ -3962,7 +3968,7 @@
         <v>42989</v>
       </c>
       <c r="B208" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C208" s="6">
         <v>29</v>
@@ -3980,7 +3986,7 @@
         <v>42990</v>
       </c>
       <c r="B209" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C209" s="7"/>
       <c r="D209" s="2"/>
@@ -3996,7 +4002,7 @@
         <v>42991</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C210" s="7"/>
       <c r="D210" s="2"/>
@@ -4012,7 +4018,7 @@
         <v>42992</v>
       </c>
       <c r="B211" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C211" s="7"/>
       <c r="D211" s="2"/>
@@ -4028,7 +4034,7 @@
         <v>42993</v>
       </c>
       <c r="B212" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C212" s="7"/>
       <c r="D212" s="2"/>
@@ -4044,7 +4050,7 @@
         <v>42994</v>
       </c>
       <c r="B213" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C213" s="8"/>
       <c r="D213" s="2"/>
@@ -4060,7 +4066,7 @@
         <v>42995</v>
       </c>
       <c r="B214" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -4076,7 +4082,7 @@
         <v>42996</v>
       </c>
       <c r="B215" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C215" s="6">
         <v>30</v>
@@ -4094,7 +4100,7 @@
         <v>42997</v>
       </c>
       <c r="B216" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C216" s="7"/>
       <c r="D216" s="2"/>
@@ -4110,7 +4116,7 @@
         <v>42998</v>
       </c>
       <c r="B217" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C217" s="7"/>
       <c r="D217" s="2"/>
@@ -4126,7 +4132,7 @@
         <v>42999</v>
       </c>
       <c r="B218" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C218" s="7"/>
       <c r="D218" s="2"/>
@@ -4142,7 +4148,7 @@
         <v>43000</v>
       </c>
       <c r="B219" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C219" s="7"/>
       <c r="D219" s="2"/>
@@ -4158,7 +4164,7 @@
         <v>43001</v>
       </c>
       <c r="B220" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C220" s="8"/>
       <c r="D220" s="2"/>
@@ -4174,7 +4180,7 @@
         <v>43002</v>
       </c>
       <c r="B221" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
@@ -4190,7 +4196,7 @@
         <v>43003</v>
       </c>
       <c r="B222" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C222" s="6">
         <v>31</v>
@@ -4208,7 +4214,7 @@
         <v>43004</v>
       </c>
       <c r="B223" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C223" s="7"/>
       <c r="D223" s="2"/>
@@ -4224,7 +4230,7 @@
         <v>43005</v>
       </c>
       <c r="B224" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C224" s="7"/>
       <c r="D224" s="2"/>
@@ -4240,7 +4246,7 @@
         <v>43006</v>
       </c>
       <c r="B225" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C225" s="7"/>
       <c r="D225" s="2"/>
@@ -4256,7 +4262,7 @@
         <v>43007</v>
       </c>
       <c r="B226" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C226" s="7"/>
       <c r="D226" s="2"/>
@@ -4272,7 +4278,7 @@
         <v>43008</v>
       </c>
       <c r="B227" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C227" s="8"/>
       <c r="D227" s="2"/>
@@ -4288,7 +4294,7 @@
         <v>43009</v>
       </c>
       <c r="B228" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -4304,7 +4310,7 @@
         <v>43010</v>
       </c>
       <c r="B229" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C229" s="6">
         <v>32</v>
@@ -4322,7 +4328,7 @@
         <v>43011</v>
       </c>
       <c r="B230" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C230" s="7"/>
       <c r="D230" s="2"/>
@@ -4338,7 +4344,7 @@
         <v>43012</v>
       </c>
       <c r="B231" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C231" s="7"/>
       <c r="D231" s="2"/>
@@ -4354,7 +4360,7 @@
         <v>43013</v>
       </c>
       <c r="B232" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C232" s="7"/>
       <c r="D232" s="2"/>
@@ -4370,7 +4376,7 @@
         <v>43014</v>
       </c>
       <c r="B233" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C233" s="7"/>
       <c r="D233" s="2"/>
@@ -4386,7 +4392,7 @@
         <v>43015</v>
       </c>
       <c r="B234" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C234" s="8"/>
       <c r="D234" s="2"/>
@@ -4402,7 +4408,7 @@
         <v>43016</v>
       </c>
       <c r="B235" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -4418,7 +4424,7 @@
         <v>43017</v>
       </c>
       <c r="B236" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C236" s="6">
         <v>33</v>
@@ -4436,7 +4442,7 @@
         <v>43018</v>
       </c>
       <c r="B237" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C237" s="7"/>
       <c r="D237" s="2"/>
@@ -4452,7 +4458,7 @@
         <v>43019</v>
       </c>
       <c r="B238" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C238" s="7"/>
       <c r="D238" s="2"/>
@@ -4468,7 +4474,7 @@
         <v>43020</v>
       </c>
       <c r="B239" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C239" s="7"/>
       <c r="D239" s="2"/>
@@ -4484,7 +4490,7 @@
         <v>43021</v>
       </c>
       <c r="B240" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C240" s="7"/>
       <c r="D240" s="2"/>
@@ -4500,7 +4506,7 @@
         <v>43022</v>
       </c>
       <c r="B241" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C241" s="8"/>
       <c r="D241" s="2"/>
@@ -4516,7 +4522,7 @@
         <v>43023</v>
       </c>
       <c r="B242" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
@@ -4532,7 +4538,7 @@
         <v>43024</v>
       </c>
       <c r="B243" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C243" s="6">
         <v>34</v>
@@ -4550,7 +4556,7 @@
         <v>43025</v>
       </c>
       <c r="B244" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C244" s="7"/>
       <c r="D244" s="2"/>
@@ -4566,7 +4572,7 @@
         <v>43026</v>
       </c>
       <c r="B245" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C245" s="7"/>
       <c r="D245" s="2"/>
@@ -4582,7 +4588,7 @@
         <v>43027</v>
       </c>
       <c r="B246" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C246" s="7"/>
       <c r="D246" s="2"/>
@@ -4598,7 +4604,7 @@
         <v>43028</v>
       </c>
       <c r="B247" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C247" s="7"/>
       <c r="D247" s="2"/>
@@ -4614,7 +4620,7 @@
         <v>43029</v>
       </c>
       <c r="B248" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C248" s="8"/>
       <c r="D248" s="2"/>
@@ -4630,7 +4636,7 @@
         <v>43030</v>
       </c>
       <c r="B249" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
@@ -4646,7 +4652,7 @@
         <v>43031</v>
       </c>
       <c r="B250" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C250" s="6">
         <v>35</v>
@@ -4664,7 +4670,7 @@
         <v>43032</v>
       </c>
       <c r="B251" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C251" s="7"/>
       <c r="D251" s="2"/>
@@ -4680,7 +4686,7 @@
         <v>43033</v>
       </c>
       <c r="B252" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C252" s="7"/>
       <c r="D252" s="2"/>
@@ -4696,7 +4702,7 @@
         <v>43034</v>
       </c>
       <c r="B253" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C253" s="7"/>
       <c r="D253" s="2"/>
@@ -4712,7 +4718,7 @@
         <v>43035</v>
       </c>
       <c r="B254" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C254" s="7"/>
       <c r="D254" s="2"/>
@@ -4728,7 +4734,7 @@
         <v>43036</v>
       </c>
       <c r="B255" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C255" s="8"/>
       <c r="D255" s="2"/>
@@ -4744,7 +4750,7 @@
         <v>43037</v>
       </c>
       <c r="B256" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
@@ -4760,7 +4766,7 @@
         <v>43038</v>
       </c>
       <c r="B257" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C257" s="6">
         <v>36</v>
@@ -4778,7 +4784,7 @@
         <v>43039</v>
       </c>
       <c r="B258" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C258" s="7"/>
       <c r="D258" s="2"/>
@@ -4794,7 +4800,7 @@
         <v>43040</v>
       </c>
       <c r="B259" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C259" s="7"/>
       <c r="D259" s="2"/>
@@ -4810,7 +4816,7 @@
         <v>43041</v>
       </c>
       <c r="B260" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C260" s="7"/>
       <c r="D260" s="2"/>
@@ -4826,7 +4832,7 @@
         <v>43042</v>
       </c>
       <c r="B261" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C261" s="7"/>
       <c r="D261" s="2"/>
@@ -4842,7 +4848,7 @@
         <v>43043</v>
       </c>
       <c r="B262" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C262" s="8"/>
       <c r="D262" s="2"/>
@@ -4858,7 +4864,7 @@
         <v>43044</v>
       </c>
       <c r="B263" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
@@ -4874,7 +4880,7 @@
         <v>43045</v>
       </c>
       <c r="B264" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C264" s="6">
         <v>37</v>
@@ -4892,7 +4898,7 @@
         <v>43046</v>
       </c>
       <c r="B265" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C265" s="7"/>
       <c r="D265" s="2"/>
@@ -4908,7 +4914,7 @@
         <v>43047</v>
       </c>
       <c r="B266" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C266" s="7"/>
       <c r="D266" s="2"/>
@@ -4924,7 +4930,7 @@
         <v>43048</v>
       </c>
       <c r="B267" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C267" s="7"/>
       <c r="D267" s="2"/>
@@ -4940,7 +4946,7 @@
         <v>43049</v>
       </c>
       <c r="B268" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C268" s="7"/>
       <c r="D268" s="2"/>
@@ -4956,7 +4962,7 @@
         <v>43050</v>
       </c>
       <c r="B269" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C269" s="8"/>
       <c r="D269" s="2"/>
@@ -4972,7 +4978,7 @@
         <v>43051</v>
       </c>
       <c r="B270" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
@@ -4988,7 +4994,7 @@
         <v>43052</v>
       </c>
       <c r="B271" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C271" s="6">
         <v>38</v>
@@ -5006,7 +5012,7 @@
         <v>43053</v>
       </c>
       <c r="B272" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C272" s="7"/>
       <c r="D272" s="2"/>
@@ -5022,7 +5028,7 @@
         <v>43054</v>
       </c>
       <c r="B273" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C273" s="7"/>
       <c r="D273" s="2"/>
@@ -5038,7 +5044,7 @@
         <v>43055</v>
       </c>
       <c r="B274" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C274" s="7"/>
       <c r="D274" s="2"/>
@@ -5054,7 +5060,7 @@
         <v>43056</v>
       </c>
       <c r="B275" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C275" s="7"/>
       <c r="D275" s="2"/>
@@ -5070,7 +5076,7 @@
         <v>43057</v>
       </c>
       <c r="B276" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C276" s="8"/>
       <c r="D276" s="2"/>
@@ -5086,7 +5092,7 @@
         <v>43058</v>
       </c>
       <c r="B277" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
@@ -5102,7 +5108,7 @@
         <v>43059</v>
       </c>
       <c r="B278" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C278" s="6">
         <v>39</v>
@@ -5120,7 +5126,7 @@
         <v>43060</v>
       </c>
       <c r="B279" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C279" s="7"/>
       <c r="D279" s="2"/>
@@ -5136,7 +5142,7 @@
         <v>43061</v>
       </c>
       <c r="B280" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C280" s="7"/>
       <c r="D280" s="2"/>
@@ -5152,7 +5158,7 @@
         <v>43062</v>
       </c>
       <c r="B281" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C281" s="7"/>
       <c r="D281" s="2"/>
@@ -5168,7 +5174,7 @@
         <v>43063</v>
       </c>
       <c r="B282" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C282" s="7"/>
       <c r="D282" s="2"/>
@@ -5184,7 +5190,7 @@
         <v>43064</v>
       </c>
       <c r="B283" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C283" s="8"/>
       <c r="D283" s="2"/>
@@ -5200,7 +5206,7 @@
         <v>43065</v>
       </c>
       <c r="B284" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
@@ -5216,7 +5222,7 @@
         <v>43066</v>
       </c>
       <c r="B285" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C285" s="6">
         <v>40</v>
@@ -5234,7 +5240,7 @@
         <v>43067</v>
       </c>
       <c r="B286" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C286" s="7"/>
       <c r="D286" s="2"/>
@@ -5250,7 +5256,7 @@
         <v>43068</v>
       </c>
       <c r="B287" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C287" s="7"/>
       <c r="D287" s="2"/>
@@ -5266,7 +5272,7 @@
         <v>43069</v>
       </c>
       <c r="B288" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C288" s="7"/>
       <c r="D288" s="2"/>
@@ -5282,7 +5288,7 @@
         <v>43070</v>
       </c>
       <c r="B289" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C289" s="7"/>
       <c r="D289" s="2"/>
@@ -5298,7 +5304,7 @@
         <v>43071</v>
       </c>
       <c r="B290" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C290" s="8"/>
       <c r="D290" s="2"/>
@@ -5314,7 +5320,7 @@
         <v>43072</v>
       </c>
       <c r="B291" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
@@ -5330,7 +5336,7 @@
         <v>43073</v>
       </c>
       <c r="B292" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C292" s="6">
         <v>41</v>
@@ -5348,7 +5354,7 @@
         <v>43074</v>
       </c>
       <c r="B293" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C293" s="7"/>
       <c r="D293" s="2"/>
@@ -5364,7 +5370,7 @@
         <v>43075</v>
       </c>
       <c r="B294" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C294" s="7"/>
       <c r="D294" s="2"/>
@@ -5380,7 +5386,7 @@
         <v>43076</v>
       </c>
       <c r="B295" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C295" s="7"/>
       <c r="D295" s="2"/>
@@ -5396,7 +5402,7 @@
         <v>43077</v>
       </c>
       <c r="B296" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C296" s="7"/>
       <c r="D296" s="2"/>
@@ -5412,7 +5418,7 @@
         <v>43078</v>
       </c>
       <c r="B297" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C297" s="8"/>
       <c r="D297" s="2"/>
@@ -5428,7 +5434,7 @@
         <v>43079</v>
       </c>
       <c r="B298" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
@@ -5444,7 +5450,7 @@
         <v>43080</v>
       </c>
       <c r="B299" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C299" s="6">
         <v>42</v>
@@ -5462,7 +5468,7 @@
         <v>43081</v>
       </c>
       <c r="B300" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C300" s="7"/>
       <c r="D300" s="2"/>
@@ -5478,7 +5484,7 @@
         <v>43082</v>
       </c>
       <c r="B301" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C301" s="7"/>
       <c r="D301" s="2"/>
@@ -5494,7 +5500,7 @@
         <v>43083</v>
       </c>
       <c r="B302" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C302" s="7"/>
       <c r="D302" s="2"/>
@@ -5510,7 +5516,7 @@
         <v>43084</v>
       </c>
       <c r="B303" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C303" s="7"/>
       <c r="D303" s="2"/>
@@ -5526,7 +5532,7 @@
         <v>43085</v>
       </c>
       <c r="B304" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C304" s="8"/>
       <c r="D304" s="2"/>
@@ -5542,7 +5548,7 @@
         <v>43086</v>
       </c>
       <c r="B305" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
@@ -5558,7 +5564,7 @@
         <v>43087</v>
       </c>
       <c r="B306" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C306" s="6">
         <v>43</v>
@@ -5576,7 +5582,7 @@
         <v>43088</v>
       </c>
       <c r="B307" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C307" s="7"/>
       <c r="D307" s="2"/>
@@ -5592,7 +5598,7 @@
         <v>43089</v>
       </c>
       <c r="B308" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C308" s="7"/>
       <c r="D308" s="2"/>
@@ -5608,7 +5614,7 @@
         <v>43090</v>
       </c>
       <c r="B309" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C309" s="7"/>
       <c r="D309" s="2"/>
@@ -5624,7 +5630,7 @@
         <v>43091</v>
       </c>
       <c r="B310" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C310" s="7"/>
       <c r="D310" s="2"/>
@@ -5640,7 +5646,7 @@
         <v>43092</v>
       </c>
       <c r="B311" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C311" s="8"/>
       <c r="D311" s="2"/>
@@ -5656,7 +5662,7 @@
         <v>43093</v>
       </c>
       <c r="B312" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
@@ -5672,7 +5678,7 @@
         <v>43094</v>
       </c>
       <c r="B313" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C313" s="6">
         <v>44</v>
@@ -5690,7 +5696,7 @@
         <v>43095</v>
       </c>
       <c r="B314" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C314" s="7"/>
       <c r="D314" s="2"/>
@@ -5706,7 +5712,7 @@
         <v>43096</v>
       </c>
       <c r="B315" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C315" s="7"/>
       <c r="D315" s="2"/>
@@ -5722,7 +5728,7 @@
         <v>43097</v>
       </c>
       <c r="B316" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C316" s="7"/>
       <c r="D316" s="2"/>
@@ -5738,7 +5744,7 @@
         <v>43098</v>
       </c>
       <c r="B317" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C317" s="7"/>
       <c r="D317" s="2"/>
@@ -5754,7 +5760,7 @@
         <v>43099</v>
       </c>
       <c r="B318" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C318" s="8"/>
       <c r="D318" s="2"/>
@@ -5770,7 +5776,7 @@
         <v>43100</v>
       </c>
       <c r="B319" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
@@ -5837,17 +5843,28 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C75:C80"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C19:C24"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="C61:C66"/>
-    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="C292:C297"/>
+    <mergeCell ref="C299:C304"/>
+    <mergeCell ref="C306:C311"/>
+    <mergeCell ref="C313:C318"/>
+    <mergeCell ref="C250:C255"/>
+    <mergeCell ref="C257:C262"/>
+    <mergeCell ref="C264:C269"/>
+    <mergeCell ref="C271:C276"/>
+    <mergeCell ref="C278:C283"/>
+    <mergeCell ref="C285:C290"/>
+    <mergeCell ref="C243:C248"/>
+    <mergeCell ref="C166:C171"/>
+    <mergeCell ref="C173:C178"/>
+    <mergeCell ref="C180:C185"/>
+    <mergeCell ref="C187:C192"/>
+    <mergeCell ref="C194:C199"/>
+    <mergeCell ref="C201:C206"/>
+    <mergeCell ref="C208:C213"/>
+    <mergeCell ref="C215:C220"/>
+    <mergeCell ref="C222:C227"/>
+    <mergeCell ref="C229:C234"/>
+    <mergeCell ref="C236:C241"/>
     <mergeCell ref="C159:C164"/>
     <mergeCell ref="C82:C87"/>
     <mergeCell ref="C89:C94"/>
@@ -5860,28 +5877,17 @@
     <mergeCell ref="C138:C143"/>
     <mergeCell ref="C145:C150"/>
     <mergeCell ref="C152:C157"/>
-    <mergeCell ref="C243:C248"/>
-    <mergeCell ref="C166:C171"/>
-    <mergeCell ref="C173:C178"/>
-    <mergeCell ref="C180:C185"/>
-    <mergeCell ref="C187:C192"/>
-    <mergeCell ref="C194:C199"/>
-    <mergeCell ref="C201:C206"/>
-    <mergeCell ref="C208:C213"/>
-    <mergeCell ref="C215:C220"/>
-    <mergeCell ref="C222:C227"/>
-    <mergeCell ref="C229:C234"/>
-    <mergeCell ref="C236:C241"/>
-    <mergeCell ref="C292:C297"/>
-    <mergeCell ref="C299:C304"/>
-    <mergeCell ref="C306:C311"/>
-    <mergeCell ref="C313:C318"/>
-    <mergeCell ref="C250:C255"/>
-    <mergeCell ref="C257:C262"/>
-    <mergeCell ref="C264:C269"/>
-    <mergeCell ref="C271:C276"/>
-    <mergeCell ref="C278:C283"/>
-    <mergeCell ref="C285:C290"/>
+    <mergeCell ref="C75:C80"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="C40:C45"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="C61:C66"/>
+    <mergeCell ref="C68:C73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>